<commit_message>
Add shadow to logos
</commit_message>
<xml_diff>
--- a/School_Data.xlsx
+++ b/School_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.boleyn\Documents\GitHub\ncaa-06-scheduler\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.boleyn\ncaa-ps2-scheduler-ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4535FE76-AC7D-45D1-9C09-B81ED0C4AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5426FC-C542-4AC5-A102-52EDFD37F88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="2925" windowWidth="21600" windowHeight="11385" xr2:uid="{AD84723E-ACBC-4464-9CF8-5905B5C1FD78}"/>
+    <workbookView xWindow="25665" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{AD84723E-ACBC-4464-9CF8-5905B5C1FD78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,9 +585,6 @@
     <t>#C5050C</t>
   </si>
   <si>
-    <t>https://teamcolorcodes.com/wisconsin-badgers-colors/#Wisconsin_Badgers_Logo_PNG</t>
-  </si>
-  <si>
     <t>Arkansas</t>
   </si>
   <si>
@@ -1035,9 +1032,6 @@
     <t>#58595B</t>
   </si>
   <si>
-    <t>https://teamcolorcodes.com/tennessee-volunteers-color-codes/#Tennessee_Volunteers_Logo_PNG</t>
-  </si>
-  <si>
     <t>Aggies</t>
   </si>
   <si>
@@ -1687,6 +1681,12 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/en/thumb/a/a6/Western_Michigan_Broncos_logo.svg/318px-Western_Michigan_Broncos_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e5/Wisconsin_Badgers_logo.svg/254px-Wisconsin_Badgers_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e3/Tennessee_Volunteers_logo.svg/240px-Tennessee_Volunteers_logo.svg.png</t>
   </si>
 </sst>
 </file>
@@ -1772,7 +1772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1847,6 +1847,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2164,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11B627A-E057-4C54-9687-7444D7F605CA}">
   <dimension ref="A1:BB1115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2235,13 +2236,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>467</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -2288,10 +2289,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>174</v>
@@ -2300,16 +2301,16 @@
         <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>118</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J2" s="13" t="s">
         <v>96</v>
@@ -2363,10 +2364,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>74</v>
@@ -2375,13 +2376,13 @@
         <v>102</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="14"/>
@@ -2434,37 +2435,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>304</v>
-      </c>
       <c r="J4" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>31</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
@@ -2513,28 +2514,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>247</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
@@ -2586,27 +2587,26 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>251</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="I6" s="15"/>
+        <v>242</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="15"/>
@@ -2656,34 +2656,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>194</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -2733,28 +2733,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>84</v>
@@ -2811,7 +2811,7 @@
         <v>118</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>120</v>
@@ -2820,16 +2820,16 @@
         <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>111</v>
@@ -2883,25 +2883,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>306</v>
-      </c>
       <c r="H10" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>38</v>
@@ -2910,7 +2910,7 @@
         <v>21</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>80</v>
@@ -2969,16 +2969,16 @@
         <v>90</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>77</v>
@@ -3033,34 +3033,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="I12" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>199</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>200</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
@@ -3110,37 +3110,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
@@ -3268,28 +3268,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -3344,22 +3344,22 @@
         <v>124</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>117</v>
@@ -3418,37 +3418,37 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="L17" s="15" t="s">
         <v>356</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="L17" s="15" t="s">
-        <v>358</v>
       </c>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
@@ -3497,28 +3497,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>256</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>99</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>94</v>
@@ -3572,31 +3572,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>57</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
@@ -3647,28 +3647,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
@@ -3804,10 +3804,10 @@
         <v>14</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>17</v>
@@ -3877,28 +3877,28 @@
         <v>174</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>154</v>
       </c>
       <c r="I23" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="J23" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -3949,31 +3949,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>174</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
@@ -4104,31 +4104,31 @@
         <v>57</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J26" s="14" t="s">
         <v>138</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
@@ -4178,7 +4178,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>65</v>
@@ -4187,19 +4187,19 @@
         <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H27" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>414</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>416</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -4254,19 +4254,19 @@
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="G28" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>18</v>
@@ -4278,10 +4278,10 @@
         <v>35</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -4406,37 +4406,37 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
@@ -4488,19 +4488,19 @@
         <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>21</v>
@@ -4509,7 +4509,7 @@
         <v>31</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>14</v>
@@ -4639,37 +4639,37 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
@@ -4718,31 +4718,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="H34" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="I34" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="J34" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>208</v>
       </c>
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
@@ -4793,13 +4793,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>39</v>
@@ -4808,13 +4808,13 @@
         <v>55</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -5103,25 +5103,25 @@
         <v>153</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>149</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>210</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>211</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>149</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>144</v>
@@ -5178,25 +5178,25 @@
         <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="12" t="s">
         <v>215</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>216</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>144</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
@@ -5248,7 +5248,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>175</v>
@@ -5257,13 +5257,13 @@
         <v>169</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="12" t="s">
         <v>218</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>219</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>169</v>
@@ -5321,28 +5321,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
@@ -5403,19 +5403,19 @@
         <v>81</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>78</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J43" s="14" t="s">
         <v>31</v>
@@ -5473,31 +5473,31 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -5625,37 +5625,37 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="H46" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="K46" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="J46" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K46" s="15" t="s">
-        <v>319</v>
-      </c>
       <c r="L46" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -5707,19 +5707,19 @@
         <v>138</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>223</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>74</v>
@@ -5728,7 +5728,7 @@
         <v>47</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K47" s="15" t="s">
         <v>57</v>
@@ -5866,19 +5866,19 @@
         <v>13</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>72</v>
@@ -5887,13 +5887,13 @@
         <v>78</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M49" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N49" s="15"/>
       <c r="O49" s="15"/>
@@ -6021,31 +6021,31 @@
         <v>77</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>72</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J51" s="14" t="s">
         <v>74</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
@@ -6248,31 +6248,31 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
@@ -6400,37 +6400,37 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="G56" s="12" t="s">
-        <v>324</v>
-      </c>
       <c r="H56" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L56" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -6561,25 +6561,25 @@
         <v>96</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G58" s="12" t="s">
         <v>350</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>352</v>
       </c>
       <c r="H58" s="13" t="s">
         <v>118</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J58" s="14" t="s">
         <v>70</v>
@@ -6591,7 +6591,7 @@
         <v>111</v>
       </c>
       <c r="M58" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N58" s="15"/>
       <c r="O58" s="15"/>
@@ -6717,28 +6717,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I60" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
@@ -6790,34 +6790,34 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="I61" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>542</v>
-      </c>
-      <c r="H61" s="13" t="s">
+      <c r="J61" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="I61" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="J61" s="14" t="s">
-        <v>365</v>
-      </c>
       <c r="K61" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -6867,28 +6867,28 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I62" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
@@ -7095,34 +7095,34 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G65" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="K65" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="H65" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="I65" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="K65" s="14" t="s">
-        <v>369</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -7172,31 +7172,31 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="H66" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="H66" s="13" t="s">
-        <v>433</v>
-      </c>
       <c r="I66" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J66" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
@@ -7247,7 +7247,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>125</v>
@@ -7256,19 +7256,19 @@
         <v>139</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I67" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J67" s="14"/>
       <c r="K67" s="14"/>
@@ -7479,19 +7479,19 @@
         <v>74</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H70" s="13" t="s">
         <v>138</v>
@@ -7627,25 +7627,25 @@
         <v>170</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="G72" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="H72" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="I72" s="13" t="s">
         <v>228</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="I72" s="13" t="s">
-        <v>229</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>154</v>
@@ -7701,28 +7701,28 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H73" s="13" t="s">
         <v>170</v>
       </c>
       <c r="I73" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J73" s="14"/>
       <c r="K73" s="14"/>
@@ -7774,37 +7774,37 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E74" s="1" t="s">
+      <c r="F74" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="G74" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="G74" s="12" t="s">
+      <c r="H74" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="I74" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="L74" s="15" t="s">
         <v>328</v>
-      </c>
-      <c r="H74" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="I74" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="J74" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K74" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="L74" s="15" t="s">
-        <v>329</v>
       </c>
       <c r="M74" s="15" t="s">
         <v>84</v>
@@ -7855,28 +7855,28 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="G75" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="G75" s="12" t="s">
+      <c r="H75" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="H75" s="13" t="s">
+      <c r="I75" s="15" t="s">
         <v>268</v>
-      </c>
-      <c r="I75" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
@@ -7928,31 +7928,31 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G76" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="I76" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="H76" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>273</v>
-      </c>
       <c r="J76" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K76" s="15"/>
       <c r="L76" s="15"/>
@@ -8242,31 +8242,31 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I80" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="I80" s="13" t="s">
+      <c r="J80" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="J80" s="14" t="s">
-        <v>208</v>
       </c>
       <c r="K80" s="15"/>
       <c r="L80" s="15"/>
@@ -8396,34 +8396,34 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G82" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="J82" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="K82" s="15" t="s">
         <v>371</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="J82" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="K82" s="15" t="s">
-        <v>373</v>
       </c>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
@@ -8472,28 +8472,28 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>160</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J83" s="14" t="s">
         <v>99</v>
@@ -8547,34 +8547,34 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J84" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L84" s="15" t="s">
         <v>96</v>
@@ -8629,19 +8629,19 @@
         <v>14</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H85" s="13" t="s">
         <v>12</v>
@@ -8703,22 +8703,22 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H86" s="13" t="s">
         <v>84</v>
@@ -8727,13 +8727,13 @@
         <v>57</v>
       </c>
       <c r="J86" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K86" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M86" s="15"/>
       <c r="N86" s="15"/>
@@ -8782,28 +8782,28 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="G87" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>435</v>
-      </c>
       <c r="H87" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
@@ -8858,28 +8858,28 @@
         <v>99</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="G88" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="G88" s="12" t="s">
-        <v>277</v>
-      </c>
       <c r="H88" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>70</v>
       </c>
       <c r="J88" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K88" s="14"/>
       <c r="L88" s="15"/>
@@ -9009,34 +9009,34 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="G90" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="G90" s="12" t="s">
+      <c r="H90" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="I90" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="J90" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="K90" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="H90" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="I90" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="J90" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="K90" s="15" t="s">
-        <v>237</v>
       </c>
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
@@ -9089,19 +9089,19 @@
         <v>106</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G91" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H91" s="13" t="s">
         <v>111</v>
@@ -9165,28 +9165,28 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E92" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="G92" s="12" t="s">
-        <v>336</v>
+        <v>553</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J92" s="14" t="s">
         <v>31</v>
@@ -9241,37 +9241,37 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G93" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H93" s="13" t="s">
         <v>170</v>
       </c>
       <c r="I93" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="K93" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="L93" s="15" t="s">
         <v>194</v>
-      </c>
-      <c r="J93" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K93" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="L93" s="15" t="s">
-        <v>195</v>
       </c>
       <c r="M93" s="15"/>
       <c r="N93" s="15"/>
@@ -9319,37 +9319,37 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G94" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J94" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K94" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L94" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
@@ -9398,13 +9398,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>54</v>
@@ -9413,16 +9413,16 @@
         <v>55</v>
       </c>
       <c r="G95" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I95" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="J95" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="J95" s="14" t="s">
-        <v>195</v>
       </c>
       <c r="K95" s="15"/>
       <c r="L95" s="15"/>
@@ -9473,28 +9473,28 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G96" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I96" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
@@ -9546,28 +9546,28 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G97" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
@@ -9619,37 +9619,37 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I98" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J98" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K98" s="15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L98" s="15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M98" s="15"/>
       <c r="N98" s="15"/>
@@ -9698,28 +9698,28 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G99" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J99" s="14" t="s">
         <v>84</v>
@@ -9773,28 +9773,28 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E100" s="1" t="s">
+      <c r="F100" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="G100" s="12" t="s">
         <v>281</v>
-      </c>
-      <c r="G100" s="12" t="s">
-        <v>282</v>
       </c>
       <c r="H100" s="13" t="s">
         <v>94</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
@@ -9923,28 +9923,28 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G102" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I102" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
@@ -9999,31 +9999,31 @@
         <v>94</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F103" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G103" s="12" t="s">
         <v>284</v>
-      </c>
-      <c r="G103" s="12" t="s">
-        <v>285</v>
       </c>
       <c r="H103" s="15" t="s">
         <v>70</v>
       </c>
       <c r="I103" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J103" s="13" t="s">
         <v>99</v>
       </c>
       <c r="K103" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L103" s="15"/>
       <c r="M103" s="15"/>
@@ -10073,28 +10073,28 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F104" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G104" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="G104" s="12" t="s">
+      <c r="H104" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="H104" s="13" t="s">
+      <c r="I104" s="13" t="s">
         <v>289</v>
-      </c>
-      <c r="I104" s="13" t="s">
-        <v>290</v>
       </c>
       <c r="J104" s="14" t="s">
         <v>174</v>
@@ -10148,31 +10148,31 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G105" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J105" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K105" s="15"/>
       <c r="L105" s="15"/>
@@ -10223,31 +10223,31 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>102</v>
       </c>
       <c r="G106" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H106" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I106" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J106" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K106" s="15"/>
       <c r="L106" s="15"/>
@@ -10298,28 +10298,28 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I107" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
@@ -10601,31 +10601,31 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E111" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="G111" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="G111" s="12" t="s">
-        <v>293</v>
-      </c>
       <c r="H111" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I111" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J111" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K111" s="15"/>
       <c r="L111" s="15"/>
@@ -10676,31 +10676,31 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E112" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="G112" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="G112" s="12" t="s">
+      <c r="H112" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="I112" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="H112" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="I112" s="13" t="s">
-        <v>297</v>
-      </c>
       <c r="J112" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K112" s="14"/>
       <c r="L112" s="15"/>
@@ -10832,28 +10832,28 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G114" s="12" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H114" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I114" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J114" s="14"/>
       <c r="K114" s="15"/>
@@ -10919,8 +10919,8 @@
       <c r="F115" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G115" s="12" t="s">
-        <v>186</v>
+      <c r="G115" s="28" t="s">
+        <v>552</v>
       </c>
       <c r="H115" s="13" t="s">
         <v>105</v>
@@ -10978,34 +10978,34 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G116" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I116" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="J116" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="K116" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="J116" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="K116" s="14" t="s">
-        <v>290</v>
       </c>
       <c r="L116" s="15"/>
       <c r="M116" s="15"/>
@@ -11055,10 +11055,10 @@
         <v>129</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>66</v>
@@ -11118,31 +11118,31 @@
         <v>143</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G118" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H118" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I118" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J118" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K118" s="14"/>
       <c r="L118" s="15"/>
@@ -11193,25 +11193,25 @@
         <v>144</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G119" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I119" s="15"/>
       <c r="J119" s="14"/>
@@ -11264,10 +11264,10 @@
         <v>179</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>36</v>
@@ -11330,7 +11330,7 @@
         <v>129</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>66</v>
@@ -11390,7 +11390,7 @@
         <v>186</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>175</v>
@@ -11453,7 +11453,7 @@
         <v>188</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>134</v>
@@ -11462,10 +11462,10 @@
         <v>24</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="13"/>
@@ -11520,10 +11520,10 @@
         <v>189</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>14</v>
@@ -11532,7 +11532,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I124" s="13"/>
       <c r="J124" s="14"/>
@@ -11585,10 +11585,10 @@
         <v>192</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>14</v>
@@ -11597,7 +11597,7 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
@@ -11650,7 +11650,7 @@
         <v>193</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>65</v>
@@ -11659,10 +11659,10 @@
         <v>38</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" s="13"/>
@@ -11717,13 +11717,13 @@
         <v>194</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -11780,10 +11780,10 @@
         <v>195</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>24</v>
@@ -11843,13 +11843,13 @@
         <v>197</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -11906,13 +11906,13 @@
         <v>199</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -11969,25 +11969,25 @@
         <v>211</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="G131" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I131" s="1"/>
       <c r="J131" s="1"/>
@@ -12040,31 +12040,31 @@
         <v>226</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E132" s="1" t="s">
+      <c r="G132" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="F132" s="1" t="s">
+      <c r="H132" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="G132" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="H132" s="13" t="s">
-        <v>441</v>
-      </c>
       <c r="I132" s="22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J132" s="22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K132" s="23"/>
       <c r="L132" s="23"/>
@@ -12115,28 +12115,28 @@
         <v>229</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G133" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I133" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J133" s="14"/>
       <c r="K133" s="14"/>
@@ -12188,7 +12188,7 @@
         <v>230</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>107</v>
@@ -12197,16 +12197,16 @@
         <v>31</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G134" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I134" s="15"/>
       <c r="J134" s="14"/>
@@ -36417,87 +36417,87 @@
     <hyperlink ref="G69" r:id="rId38" xr:uid="{99A023F2-4507-467D-8DAB-BEB7693CC468}"/>
     <hyperlink ref="G77" r:id="rId39" xr:uid="{3E741944-62DF-4B40-9AB3-FD74FA4797F1}"/>
     <hyperlink ref="G79" r:id="rId40" xr:uid="{42B3C4A7-E66A-46C9-9258-D4BD00021921}"/>
-    <hyperlink ref="G115" r:id="rId41" location="Wisconsin_Badgers_Logo_PNG" xr:uid="{D9416004-7DE9-49D1-819F-D98E12AFC0EE}"/>
-    <hyperlink ref="G4" r:id="rId42" xr:uid="{395ABA04-AE94-40E4-A747-26C098FB7678}"/>
-    <hyperlink ref="G5" r:id="rId43" xr:uid="{2F7C5843-B6E2-4A70-B77C-E0B25C7E722E}"/>
-    <hyperlink ref="G31" r:id="rId44" xr:uid="{3A20DD7E-DA2C-47BD-8A98-21BE4CE0CA01}"/>
-    <hyperlink ref="G34" r:id="rId45" xr:uid="{86028A57-87EB-4F30-AB5F-408BC93C91CD}"/>
-    <hyperlink ref="G7" r:id="rId46" xr:uid="{6B22DC29-5E4E-489E-8EE9-B999348A2EE4}"/>
-    <hyperlink ref="G73" r:id="rId47" xr:uid="{2D2084C0-3FBA-4BF3-A816-6B7E5C574536}"/>
-    <hyperlink ref="G90" r:id="rId48" xr:uid="{1D570B06-88E2-409F-84FC-3D01A21B53FF}"/>
-    <hyperlink ref="G93" r:id="rId49" xr:uid="{956F3549-2E44-4AF1-9D53-0B1F9EF53684}"/>
-    <hyperlink ref="G95" r:id="rId50" xr:uid="{5E70A809-7D84-4A32-B45D-DECEB0E92117}"/>
-    <hyperlink ref="G10" r:id="rId51" xr:uid="{C2BE4FDC-0B85-4459-BA6C-A75AFFAC3547}"/>
-    <hyperlink ref="G6" r:id="rId52" xr:uid="{46F76A59-196E-49AD-9A97-78E4E5C31EB0}"/>
-    <hyperlink ref="G18" r:id="rId53" xr:uid="{43DD45FB-8A83-401A-88A5-B45573491AED}"/>
-    <hyperlink ref="G74" r:id="rId54" xr:uid="{F31F2BCF-6F0B-4FD5-BD21-19A524C163D9}"/>
-    <hyperlink ref="G75" r:id="rId55" xr:uid="{704B4E01-6CAB-4DF6-ACBA-A33544AD4CE0}"/>
-    <hyperlink ref="G56" r:id="rId56" xr:uid="{2A84C643-2E9D-4574-87DD-BE047174380C}"/>
-    <hyperlink ref="G28" r:id="rId57" xr:uid="{EF641F3A-F21F-480D-8ECD-EAB8C3FED787}"/>
-    <hyperlink ref="G23" r:id="rId58" xr:uid="{DD2A5884-DB10-45A9-BA26-84E0E05A1F3D}"/>
-    <hyperlink ref="G76" r:id="rId59" xr:uid="{57E61A04-606E-4446-8CF3-66D0E52E7DD5}"/>
-    <hyperlink ref="G88" r:id="rId60" xr:uid="{162D1EF2-1882-4F28-9834-DA5123BB4004}"/>
-    <hyperlink ref="G100" r:id="rId61" xr:uid="{A918A69D-90FD-4575-89F6-BF715138F13D}"/>
-    <hyperlink ref="G104" r:id="rId62" xr:uid="{FC89A150-04FD-4CA2-9979-4AC96A659200}"/>
-    <hyperlink ref="G103" r:id="rId63" xr:uid="{440B6CB8-F72E-4FC7-B619-D550263D55B3}"/>
-    <hyperlink ref="G111" r:id="rId64" xr:uid="{2CABEEBF-083A-481E-ACC6-58610BA24B97}"/>
-    <hyperlink ref="G112" r:id="rId65" xr:uid="{95075E14-BFAC-4762-80D8-14DAC7814EED}"/>
-    <hyperlink ref="G85" r:id="rId66" xr:uid="{B8133EA8-CB11-470C-BD8A-0918DED45540}"/>
-    <hyperlink ref="G92" r:id="rId67" location="Tennessee_Volunteers_Logo_PNG" xr:uid="{F19006C5-3D63-426E-AF22-F94EAAC5D92F}"/>
-    <hyperlink ref="G94" r:id="rId68" xr:uid="{0ED3021E-B9FC-4222-9DFD-4C461E64646E}"/>
-    <hyperlink ref="G107" r:id="rId69" xr:uid="{F09EEC3A-A27D-42BF-926D-B74B608B6982}"/>
-    <hyperlink ref="G47" r:id="rId70" xr:uid="{CAD326C2-2D39-48E2-B346-1ECC6344C2AC}"/>
-    <hyperlink ref="G132" r:id="rId71" xr:uid="{AFF9A11F-0391-45EC-96ED-DACA95F9F655}"/>
-    <hyperlink ref="G9" r:id="rId72" xr:uid="{C5BC2CC9-9D46-425E-98F2-EB4A4EE17372}"/>
-    <hyperlink ref="G16" r:id="rId73" xr:uid="{B145F603-B33F-4198-9F3E-9BCEF1DCF8E1}"/>
-    <hyperlink ref="G97" r:id="rId74" xr:uid="{C168A749-B084-4583-A0C9-63104DBFC00B}"/>
-    <hyperlink ref="G13" r:id="rId75" xr:uid="{8B20DACA-D7A5-417E-B267-101248971D20}"/>
-    <hyperlink ref="G2" r:id="rId76" xr:uid="{92616F7C-9B03-41D9-8F83-1CEAD9503033}"/>
-    <hyperlink ref="G24" r:id="rId77" xr:uid="{8AD422B7-FEC5-4213-8068-E0AF7FE7F633}"/>
-    <hyperlink ref="G30" r:id="rId78" xr:uid="{EB5B3FA5-C283-4E2F-BDF3-56A4E1DEF69A}"/>
-    <hyperlink ref="G83" r:id="rId79" xr:uid="{ED26E1A2-5080-4646-BBC8-69879871671F}"/>
-    <hyperlink ref="G82" r:id="rId80" xr:uid="{730AACE5-2C28-4F34-B8AB-A39A8EC56B0F}"/>
-    <hyperlink ref="G105" r:id="rId81" xr:uid="{93490068-C14A-43CF-B67F-E3ADA0A5197E}"/>
-    <hyperlink ref="G116" r:id="rId82" xr:uid="{C8C6DD4F-8AC2-4095-A1C7-06C0C3876197}"/>
-    <hyperlink ref="G35" r:id="rId83" xr:uid="{EA982AD7-B70D-4955-9F03-8A82F72ED889}"/>
-    <hyperlink ref="G17" r:id="rId84" xr:uid="{6E6B1EBB-61CE-4C4F-BE4D-008732A3DCDB}"/>
-    <hyperlink ref="G54" r:id="rId85" xr:uid="{471EF40F-D3BE-49F7-98DC-39DE9E1C3924}"/>
-    <hyperlink ref="G131" r:id="rId86" xr:uid="{CE3814B3-CE92-43C4-9D91-05D5A315B303}"/>
-    <hyperlink ref="G11" r:id="rId87" xr:uid="{C5F7D73F-59DE-4A1D-B0B1-87952A20C4DD}"/>
-    <hyperlink ref="G67" r:id="rId88" xr:uid="{D846212A-A585-4410-AFE5-E51B0BBC244E}"/>
-    <hyperlink ref="G70" r:id="rId89" xr:uid="{4229EFC9-0928-46EF-AAE4-44D6C22B6954}"/>
-    <hyperlink ref="G51" r:id="rId90" xr:uid="{8E0F137D-F887-492B-8022-DE208773DDFD}"/>
-    <hyperlink ref="G86" r:id="rId91" xr:uid="{4B246887-CC0E-48F5-8BDE-0DDEF7E39C25}"/>
-    <hyperlink ref="G87" r:id="rId92" xr:uid="{75173C3C-AAF9-4864-B109-966FB050D9FF}"/>
-    <hyperlink ref="G66" r:id="rId93" xr:uid="{B444BC1D-D6D1-492C-8898-B1F8BB4D2F15}"/>
-    <hyperlink ref="G49" r:id="rId94" xr:uid="{33388A3A-4EAC-4CE0-8D7B-91316BBCC0F2}"/>
-    <hyperlink ref="G42" r:id="rId95" xr:uid="{C2CE1D26-DBCC-4DFA-BEE8-4806F8A1C8A2}"/>
-    <hyperlink ref="G3" r:id="rId96" xr:uid="{2F7C6C4E-1445-4487-B601-CD5A8A79383E}"/>
-    <hyperlink ref="G15" r:id="rId97" xr:uid="{7222D6C3-7D27-447E-849E-F8246040B563}"/>
-    <hyperlink ref="G96" r:id="rId98" xr:uid="{7AB79E9B-0F3F-42C8-95F1-DCB935DBD100}"/>
-    <hyperlink ref="G26" r:id="rId99" xr:uid="{A18D4BCA-53EE-48FB-A752-D109B638BE8A}"/>
-    <hyperlink ref="G33" r:id="rId100" xr:uid="{FB7339B0-D8F3-4738-8BE2-140199AEA655}"/>
-    <hyperlink ref="G98" r:id="rId101" xr:uid="{58569C3D-CA82-4908-A49F-BEEBD70D51DB}"/>
-    <hyperlink ref="G65" r:id="rId102" xr:uid="{B4FF6E25-2F8E-44EB-92B3-3013D96B5789}"/>
-    <hyperlink ref="G8" r:id="rId103" xr:uid="{3EDC6A8C-BDA0-4E78-AFF2-E18EC7B8E5BC}"/>
-    <hyperlink ref="G20" r:id="rId104" xr:uid="{DEFB8E46-A145-4585-B280-F5181159D405}"/>
-    <hyperlink ref="G27" r:id="rId105" xr:uid="{AC730625-1130-4C7A-8DD5-82B6B102BA94}"/>
-    <hyperlink ref="G133" r:id="rId106" xr:uid="{DCF5C696-2FE7-443D-A084-C6941CE73BC9}"/>
-    <hyperlink ref="G134" r:id="rId107" xr:uid="{8B2D127D-82C9-44FE-B19A-7F0AC7C9EFED}"/>
-    <hyperlink ref="G44" r:id="rId108" xr:uid="{B2FF31FD-E675-4CF7-8D32-BD9784C36F07}"/>
-    <hyperlink ref="G60" r:id="rId109" xr:uid="{845ADDC5-3216-4B3D-AD9D-0C966999709D}"/>
-    <hyperlink ref="G61" r:id="rId110" xr:uid="{7BA9C4AD-766E-47C5-849F-F4586D8FCD35}"/>
-    <hyperlink ref="G62" r:id="rId111" xr:uid="{D2952CCD-5299-44C9-B8F5-D00C8F8E0076}"/>
-    <hyperlink ref="G80" r:id="rId112" xr:uid="{F31FC38B-5E7F-429A-8523-BEDCFCF84D15}"/>
-    <hyperlink ref="G84" r:id="rId113" xr:uid="{C5F4F8ED-E0A2-4BD3-8414-FE6FED8185E4}"/>
-    <hyperlink ref="G91" r:id="rId114" xr:uid="{9C313FC9-DD00-45A2-A9EF-A1C9B6359676}"/>
-    <hyperlink ref="G118" r:id="rId115" xr:uid="{92B93D58-272D-46BC-AC40-E853657B4F1B}"/>
-    <hyperlink ref="G99" r:id="rId116" xr:uid="{C8E197EE-EE7A-4DFC-B14B-4099E939194B}"/>
-    <hyperlink ref="G19" r:id="rId117" xr:uid="{11E39234-3172-4B6C-9DE6-922A56FEF41D}"/>
-    <hyperlink ref="G102" r:id="rId118" xr:uid="{088E929A-5754-4AE8-A132-E1FCEB68361A}"/>
-    <hyperlink ref="G119" r:id="rId119" xr:uid="{F578FDEC-E600-455F-B1A0-8B4F32E181BA}"/>
-    <hyperlink ref="G106" r:id="rId120" xr:uid="{7B5FF705-AD83-45F8-9623-E9BEDA2CB285}"/>
-    <hyperlink ref="G114" r:id="rId121" xr:uid="{19AD7DFA-DD1B-4932-A9FB-B9DF1FF0C21D}"/>
+    <hyperlink ref="G4" r:id="rId41" xr:uid="{395ABA04-AE94-40E4-A747-26C098FB7678}"/>
+    <hyperlink ref="G5" r:id="rId42" xr:uid="{2F7C5843-B6E2-4A70-B77C-E0B25C7E722E}"/>
+    <hyperlink ref="G31" r:id="rId43" xr:uid="{3A20DD7E-DA2C-47BD-8A98-21BE4CE0CA01}"/>
+    <hyperlink ref="G34" r:id="rId44" xr:uid="{86028A57-87EB-4F30-AB5F-408BC93C91CD}"/>
+    <hyperlink ref="G7" r:id="rId45" xr:uid="{6B22DC29-5E4E-489E-8EE9-B999348A2EE4}"/>
+    <hyperlink ref="G73" r:id="rId46" xr:uid="{2D2084C0-3FBA-4BF3-A816-6B7E5C574536}"/>
+    <hyperlink ref="G90" r:id="rId47" xr:uid="{1D570B06-88E2-409F-84FC-3D01A21B53FF}"/>
+    <hyperlink ref="G93" r:id="rId48" xr:uid="{956F3549-2E44-4AF1-9D53-0B1F9EF53684}"/>
+    <hyperlink ref="G95" r:id="rId49" xr:uid="{5E70A809-7D84-4A32-B45D-DECEB0E92117}"/>
+    <hyperlink ref="G10" r:id="rId50" xr:uid="{C2BE4FDC-0B85-4459-BA6C-A75AFFAC3547}"/>
+    <hyperlink ref="G6" r:id="rId51" xr:uid="{46F76A59-196E-49AD-9A97-78E4E5C31EB0}"/>
+    <hyperlink ref="G18" r:id="rId52" xr:uid="{43DD45FB-8A83-401A-88A5-B45573491AED}"/>
+    <hyperlink ref="G74" r:id="rId53" xr:uid="{F31F2BCF-6F0B-4FD5-BD21-19A524C163D9}"/>
+    <hyperlink ref="G75" r:id="rId54" xr:uid="{704B4E01-6CAB-4DF6-ACBA-A33544AD4CE0}"/>
+    <hyperlink ref="G56" r:id="rId55" xr:uid="{2A84C643-2E9D-4574-87DD-BE047174380C}"/>
+    <hyperlink ref="G28" r:id="rId56" xr:uid="{EF641F3A-F21F-480D-8ECD-EAB8C3FED787}"/>
+    <hyperlink ref="G23" r:id="rId57" xr:uid="{DD2A5884-DB10-45A9-BA26-84E0E05A1F3D}"/>
+    <hyperlink ref="G76" r:id="rId58" xr:uid="{57E61A04-606E-4446-8CF3-66D0E52E7DD5}"/>
+    <hyperlink ref="G88" r:id="rId59" xr:uid="{162D1EF2-1882-4F28-9834-DA5123BB4004}"/>
+    <hyperlink ref="G100" r:id="rId60" xr:uid="{A918A69D-90FD-4575-89F6-BF715138F13D}"/>
+    <hyperlink ref="G104" r:id="rId61" xr:uid="{FC89A150-04FD-4CA2-9979-4AC96A659200}"/>
+    <hyperlink ref="G103" r:id="rId62" xr:uid="{440B6CB8-F72E-4FC7-B619-D550263D55B3}"/>
+    <hyperlink ref="G111" r:id="rId63" xr:uid="{2CABEEBF-083A-481E-ACC6-58610BA24B97}"/>
+    <hyperlink ref="G112" r:id="rId64" xr:uid="{95075E14-BFAC-4762-80D8-14DAC7814EED}"/>
+    <hyperlink ref="G85" r:id="rId65" xr:uid="{B8133EA8-CB11-470C-BD8A-0918DED45540}"/>
+    <hyperlink ref="G92" r:id="rId66" xr:uid="{F19006C5-3D63-426E-AF22-F94EAAC5D92F}"/>
+    <hyperlink ref="G94" r:id="rId67" xr:uid="{0ED3021E-B9FC-4222-9DFD-4C461E64646E}"/>
+    <hyperlink ref="G107" r:id="rId68" xr:uid="{F09EEC3A-A27D-42BF-926D-B74B608B6982}"/>
+    <hyperlink ref="G47" r:id="rId69" xr:uid="{CAD326C2-2D39-48E2-B346-1ECC6344C2AC}"/>
+    <hyperlink ref="G132" r:id="rId70" xr:uid="{AFF9A11F-0391-45EC-96ED-DACA95F9F655}"/>
+    <hyperlink ref="G9" r:id="rId71" xr:uid="{C5BC2CC9-9D46-425E-98F2-EB4A4EE17372}"/>
+    <hyperlink ref="G16" r:id="rId72" xr:uid="{B145F603-B33F-4198-9F3E-9BCEF1DCF8E1}"/>
+    <hyperlink ref="G97" r:id="rId73" xr:uid="{C168A749-B084-4583-A0C9-63104DBFC00B}"/>
+    <hyperlink ref="G13" r:id="rId74" xr:uid="{8B20DACA-D7A5-417E-B267-101248971D20}"/>
+    <hyperlink ref="G2" r:id="rId75" xr:uid="{92616F7C-9B03-41D9-8F83-1CEAD9503033}"/>
+    <hyperlink ref="G24" r:id="rId76" xr:uid="{8AD422B7-FEC5-4213-8068-E0AF7FE7F633}"/>
+    <hyperlink ref="G30" r:id="rId77" xr:uid="{EB5B3FA5-C283-4E2F-BDF3-56A4E1DEF69A}"/>
+    <hyperlink ref="G83" r:id="rId78" xr:uid="{ED26E1A2-5080-4646-BBC8-69879871671F}"/>
+    <hyperlink ref="G82" r:id="rId79" xr:uid="{730AACE5-2C28-4F34-B8AB-A39A8EC56B0F}"/>
+    <hyperlink ref="G105" r:id="rId80" xr:uid="{93490068-C14A-43CF-B67F-E3ADA0A5197E}"/>
+    <hyperlink ref="G116" r:id="rId81" xr:uid="{C8C6DD4F-8AC2-4095-A1C7-06C0C3876197}"/>
+    <hyperlink ref="G35" r:id="rId82" xr:uid="{EA982AD7-B70D-4955-9F03-8A82F72ED889}"/>
+    <hyperlink ref="G17" r:id="rId83" xr:uid="{6E6B1EBB-61CE-4C4F-BE4D-008732A3DCDB}"/>
+    <hyperlink ref="G54" r:id="rId84" xr:uid="{471EF40F-D3BE-49F7-98DC-39DE9E1C3924}"/>
+    <hyperlink ref="G131" r:id="rId85" xr:uid="{CE3814B3-CE92-43C4-9D91-05D5A315B303}"/>
+    <hyperlink ref="G11" r:id="rId86" xr:uid="{C5F7D73F-59DE-4A1D-B0B1-87952A20C4DD}"/>
+    <hyperlink ref="G67" r:id="rId87" xr:uid="{D846212A-A585-4410-AFE5-E51B0BBC244E}"/>
+    <hyperlink ref="G70" r:id="rId88" xr:uid="{4229EFC9-0928-46EF-AAE4-44D6C22B6954}"/>
+    <hyperlink ref="G51" r:id="rId89" xr:uid="{8E0F137D-F887-492B-8022-DE208773DDFD}"/>
+    <hyperlink ref="G86" r:id="rId90" xr:uid="{4B246887-CC0E-48F5-8BDE-0DDEF7E39C25}"/>
+    <hyperlink ref="G87" r:id="rId91" xr:uid="{75173C3C-AAF9-4864-B109-966FB050D9FF}"/>
+    <hyperlink ref="G66" r:id="rId92" xr:uid="{B444BC1D-D6D1-492C-8898-B1F8BB4D2F15}"/>
+    <hyperlink ref="G49" r:id="rId93" xr:uid="{33388A3A-4EAC-4CE0-8D7B-91316BBCC0F2}"/>
+    <hyperlink ref="G42" r:id="rId94" xr:uid="{C2CE1D26-DBCC-4DFA-BEE8-4806F8A1C8A2}"/>
+    <hyperlink ref="G3" r:id="rId95" xr:uid="{2F7C6C4E-1445-4487-B601-CD5A8A79383E}"/>
+    <hyperlink ref="G15" r:id="rId96" xr:uid="{7222D6C3-7D27-447E-849E-F8246040B563}"/>
+    <hyperlink ref="G96" r:id="rId97" xr:uid="{7AB79E9B-0F3F-42C8-95F1-DCB935DBD100}"/>
+    <hyperlink ref="G26" r:id="rId98" xr:uid="{A18D4BCA-53EE-48FB-A752-D109B638BE8A}"/>
+    <hyperlink ref="G33" r:id="rId99" xr:uid="{FB7339B0-D8F3-4738-8BE2-140199AEA655}"/>
+    <hyperlink ref="G98" r:id="rId100" xr:uid="{58569C3D-CA82-4908-A49F-BEEBD70D51DB}"/>
+    <hyperlink ref="G65" r:id="rId101" xr:uid="{B4FF6E25-2F8E-44EB-92B3-3013D96B5789}"/>
+    <hyperlink ref="G8" r:id="rId102" xr:uid="{3EDC6A8C-BDA0-4E78-AFF2-E18EC7B8E5BC}"/>
+    <hyperlink ref="G20" r:id="rId103" xr:uid="{DEFB8E46-A145-4585-B280-F5181159D405}"/>
+    <hyperlink ref="G27" r:id="rId104" xr:uid="{AC730625-1130-4C7A-8DD5-82B6B102BA94}"/>
+    <hyperlink ref="G133" r:id="rId105" xr:uid="{DCF5C696-2FE7-443D-A084-C6941CE73BC9}"/>
+    <hyperlink ref="G134" r:id="rId106" xr:uid="{8B2D127D-82C9-44FE-B19A-7F0AC7C9EFED}"/>
+    <hyperlink ref="G44" r:id="rId107" xr:uid="{B2FF31FD-E675-4CF7-8D32-BD9784C36F07}"/>
+    <hyperlink ref="G60" r:id="rId108" xr:uid="{845ADDC5-3216-4B3D-AD9D-0C966999709D}"/>
+    <hyperlink ref="G61" r:id="rId109" xr:uid="{7BA9C4AD-766E-47C5-849F-F4586D8FCD35}"/>
+    <hyperlink ref="G62" r:id="rId110" xr:uid="{D2952CCD-5299-44C9-B8F5-D00C8F8E0076}"/>
+    <hyperlink ref="G80" r:id="rId111" xr:uid="{F31FC38B-5E7F-429A-8523-BEDCFCF84D15}"/>
+    <hyperlink ref="G84" r:id="rId112" xr:uid="{C5F4F8ED-E0A2-4BD3-8414-FE6FED8185E4}"/>
+    <hyperlink ref="G91" r:id="rId113" xr:uid="{9C313FC9-DD00-45A2-A9EF-A1C9B6359676}"/>
+    <hyperlink ref="G118" r:id="rId114" xr:uid="{92B93D58-272D-46BC-AC40-E853657B4F1B}"/>
+    <hyperlink ref="G99" r:id="rId115" xr:uid="{C8E197EE-EE7A-4DFC-B14B-4099E939194B}"/>
+    <hyperlink ref="G19" r:id="rId116" xr:uid="{11E39234-3172-4B6C-9DE6-922A56FEF41D}"/>
+    <hyperlink ref="G102" r:id="rId117" xr:uid="{088E929A-5754-4AE8-A132-E1FCEB68361A}"/>
+    <hyperlink ref="G119" r:id="rId118" xr:uid="{F578FDEC-E600-455F-B1A0-8B4F32E181BA}"/>
+    <hyperlink ref="G106" r:id="rId119" xr:uid="{7B5FF705-AD83-45F8-9623-E9BEDA2CB285}"/>
+    <hyperlink ref="G114" r:id="rId120" xr:uid="{19AD7DFA-DD1B-4932-A9FB-B9DF1FF0C21D}"/>
+    <hyperlink ref="G115" r:id="rId121" xr:uid="{C77B0825-6A35-44D8-950A-3EFFEC728354}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId122"/>

</xml_diff>